<commit_message>
Details added about the Contributors
</commit_message>
<xml_diff>
--- a/00_ProjectManagement/Jobs.xlsx
+++ b/00_ProjectManagement/Jobs.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
   <si>
     <t>Sr No</t>
   </si>
@@ -76,13 +76,55 @@
     <t>Project Management
 Requirements
 Dev and V</t>
+  </si>
+  <si>
+    <t>Prajwala Pandit</t>
+  </si>
+  <si>
+    <t>Requirements
+Ana and design
+Dev and V</t>
+  </si>
+  <si>
+    <t>Payal Shah</t>
+  </si>
+  <si>
+    <t>Ana and design
+Development and Ver</t>
+  </si>
+  <si>
+    <t>Harsimran singh</t>
+  </si>
+  <si>
+    <t>controller and DSP</t>
+  </si>
+  <si>
+    <t>Bharat Bansal</t>
+  </si>
+  <si>
+    <t>Controller &amp; client app</t>
+  </si>
+  <si>
+    <t>Analysis and design , Dev</t>
+  </si>
+  <si>
+    <t>Danish Ahmed</t>
+  </si>
+  <si>
+    <t>Raghuraj</t>
+  </si>
+  <si>
+    <t>Analysis and Design, Development and verification</t>
+  </si>
+  <si>
+    <t>Adit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +148,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12.1"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12.1"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -115,7 +178,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -123,17 +186,46 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -433,20 +525,20 @@
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="18.75">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="19.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -463,24 +555,120 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="45">
-      <c r="A2">
+    <row r="2" spans="1:11" ht="63.75" thickBot="1">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="3">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:11">
+    <row r="3" spans="1:11" ht="48" thickBot="1">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="48" thickBot="1">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="48" thickBot="1">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="16.5" thickBot="1">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="3">
+        <v>5</v>
+      </c>
       <c r="J8" t="s">
         <v>16</v>
       </c>
@@ -488,7 +676,22 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11">
+    <row r="9" spans="1:11" ht="48" thickBot="1">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3">
+        <v>5</v>
+      </c>
       <c r="J9" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
added fields, roles, hours per week
</commit_message>
<xml_diff>
--- a/00_ProjectManagement/Jobs.xlsx
+++ b/00_ProjectManagement/Jobs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="7185"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
   <si>
     <t>Sr No</t>
   </si>
@@ -118,13 +118,19 @@
   </si>
   <si>
     <t>Adit</t>
+  </si>
+  <si>
+    <t>Ganesh R</t>
+  </si>
+  <si>
+    <t>Development, Validation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -178,7 +184,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -201,16 +207,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -228,12 +242,24 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -312,6 +338,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -346,6 +373,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -521,24 +549,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" customWidth="1"/>
     <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="19.5" thickBot="1">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -555,185 +583,200 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="63.75" thickBot="1">
-      <c r="A2" s="3">
+    <row r="2" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="2">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="48" thickBot="1">
-      <c r="A3" s="6">
+    <row r="3" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="48" thickBot="1">
-      <c r="A4" s="6">
+    <row r="4" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
         <v>3</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A5" s="6">
+    <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
         <v>4</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-    </row>
-    <row r="6" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A6" s="6">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1">
-      <c r="A7" s="6">
+    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5" thickBot="1">
-      <c r="A8" s="3">
+    <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>5</v>
       </c>
       <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="48" thickBot="1">
-      <c r="A9" s="3">
+    <row r="9" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>5</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="2"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="K9" s="9"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
       <c r="J10" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="2"/>
-    </row>
-    <row r="11" spans="1:11">
+      <c r="K10" s="9"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J11" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="2"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="K11" s="9"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J12" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="2"/>
-    </row>
-    <row r="15" spans="1:11">
+      <c r="K12" s="9"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="9" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="2"/>
-    </row>
-    <row r="17" spans="10:11">
+      <c r="K16" s="9"/>
+    </row>
+    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -746,24 +789,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Hours and Task information updated !
</commit_message>
<xml_diff>
--- a/00_ProjectManagement/Jobs.xlsx
+++ b/00_ProjectManagement/Jobs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="7185"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
     <t>Sr No</t>
   </si>
@@ -124,13 +124,18 @@
   </si>
   <si>
     <t>Development, Validation</t>
+  </si>
+  <si>
+    <t>Project Management Requirements
+Ana and design
+Dev and V</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -242,13 +247,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -338,7 +343,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -373,7 +377,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -549,14 +552,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10.140625" customWidth="1"/>
     <col min="2" max="2" width="16.28515625" bestFit="1" customWidth="1"/>
@@ -566,7 +569,7 @@
     <col min="10" max="10" width="28.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="1" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="19.5" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="63.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="48" thickBot="1">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -600,7 +603,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="48" thickBot="1">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -617,7 +620,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="32.25" thickBot="1">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -634,7 +637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="16.5" thickBot="1">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -647,7 +650,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="16.5" thickBot="1">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -664,7 +667,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="32.25" thickBot="1">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -681,7 +684,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="16.5" thickBot="1">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -700,11 +703,11 @@
       <c r="J8" t="s">
         <v>16</v>
       </c>
-      <c r="K8" s="9" t="s">
+      <c r="K8" s="11" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="48" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="63.75" thickBot="1">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -715,24 +718,24 @@
         <v>25</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="E9" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
         <v>13</v>
       </c>
-      <c r="K9" s="9"/>
-    </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="10">
+      <c r="K9" s="11"/>
+    </row>
+    <row r="10" spans="1:11" ht="15.75">
+      <c r="A10" s="9">
         <v>9</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D10" t="s">
@@ -744,39 +747,39 @@
       <c r="J10" t="s">
         <v>7</v>
       </c>
-      <c r="K10" s="9"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K10" s="11"/>
+    </row>
+    <row r="11" spans="1:11">
       <c r="J11" t="s">
         <v>8</v>
       </c>
-      <c r="K11" s="9"/>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K11" s="11"/>
+    </row>
+    <row r="12" spans="1:11">
       <c r="J12" t="s">
         <v>9</v>
       </c>
-      <c r="K12" s="9"/>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K12" s="11"/>
+    </row>
+    <row r="15" spans="1:11">
       <c r="J15" t="s">
         <v>10</v>
       </c>
-      <c r="K15" s="9" t="s">
+      <c r="K15" s="11" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11">
       <c r="J16" t="s">
         <v>11</v>
       </c>
-      <c r="K16" s="9"/>
-    </row>
-    <row r="17" spans="10:11" x14ac:dyDescent="0.25">
+      <c r="K16" s="11"/>
+    </row>
+    <row r="17" spans="10:11">
       <c r="J17" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="9"/>
+      <c r="K17" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -789,24 +792,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>